<commit_message>
Update to print out
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BenLevinson/Documents/Senior_Year/IEMS313/Project/IEMS-Phase-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6F2BCC-8F2B-2A4B-8428-5C5F80421BDB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D13099-08CC-AA46-82C0-62F44C712336}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27380" yWindow="11380" windowWidth="26840" windowHeight="15940" xr2:uid="{16C587C2-60D2-AA43-B7AD-2ED031E7887C}"/>
+    <workbookView xWindow="32060" yWindow="15680" windowWidth="26840" windowHeight="15940" xr2:uid="{16C587C2-60D2-AA43-B7AD-2ED031E7887C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="small_instance1" localSheetId="0">Sheet1!$A$2:$C$22</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{9CB303D3-60F8-BC4A-A307-0E116C2C5233}" name="small_instance1" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/BenLevinson/Documents/Senior_Year/IEMS313/Project/IEMS-Phase-1/small_instance1.txt" delimited="0">
+    <textPr sourceFile="/Users/BenLevinson/Documents/Senior_Year/IEMS313/Project/IEMS-Phase-1/small_instance1.txt" delimited="0">
       <textFields count="3">
         <textField/>
         <textField position="2"/>
@@ -39,10 +39,6 @@
     </textPr>
   </connection>
 </connections>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -399,7 +395,7 @@
   <dimension ref="A2:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -469,13 +465,14 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>